<commit_message>
ProductCards, UpdatingCart, PlacingOrder test cases
</commit_message>
<xml_diff>
--- a/aqa-inforce-testcases.xlsx
+++ b/aqa-inforce-testcases.xlsx
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\aqa-inforce-anton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC176E85-E337-4A5B-904D-808D59E3D91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1291ABCE-262E-4132-89B9-47D8C3C16C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17520" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TC01_Categories" sheetId="1" r:id="rId1"/>
-    <sheet name="TC02_Pages" sheetId="2" r:id="rId2"/>
+    <sheet name="TC00_Empty" sheetId="3" r:id="rId1"/>
+    <sheet name="TC01_Categories" sheetId="1" r:id="rId2"/>
+    <sheet name="TC02_Pages" sheetId="2" r:id="rId3"/>
+    <sheet name="TC03_ProductCards" sheetId="4" r:id="rId4"/>
+    <sheet name="TC04_UpdatingCart" sheetId="5" r:id="rId5"/>
+    <sheet name="TC05_PlacingOrder" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -162,6 +166,87 @@
   </si>
   <si>
     <t>Shows previous page of a product cards. "Next" button appears</t>
+  </si>
+  <si>
+    <t>Pressing at any product card opens details description</t>
+  </si>
+  <si>
+    <t>Press at any product card. For example: "Apple Monitor 24"</t>
+  </si>
+  <si>
+    <t>Shows detailed description. Shows "Add to Cart" button</t>
+  </si>
+  <si>
+    <t>Click at any product card. For example "Samsung Galaxy S6"</t>
+  </si>
+  <si>
+    <t>Click "Add to cart" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows a windows with text "Product added" </t>
+  </si>
+  <si>
+    <t>Click "Add to cart" button 2 times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At every click it shows a windows with text "Product added" </t>
+  </si>
+  <si>
+    <t>Opens "Main Page" of website</t>
+  </si>
+  <si>
+    <t>Click at any other product card. For example "Nexus 6"</t>
+  </si>
+  <si>
+    <t>Click "Add to cart" button 1 times</t>
+  </si>
+  <si>
+    <t>Click "Home" button at navigational panel</t>
+  </si>
+  <si>
+    <t>Click "Cart" button at navigational panel</t>
+  </si>
+  <si>
+    <t>Deleting and adding products to the cart show changes at the cart page</t>
+  </si>
+  <si>
+    <t>Product deleted and total price changed correctly</t>
+  </si>
+  <si>
+    <t>Placing order of the products at the "Cart" page</t>
+  </si>
+  <si>
+    <t>Shows a product table with added "Samsung Galaxy S6" card. Table shows price of the picture, title, price and "Delete" button. At the right of the table there is a Total Price with button "Place Order</t>
+  </si>
+  <si>
+    <t>Shows a product table with added 3 cards. Table shows price of the picture, title, price and "Delete" button. At the right of the table there is a Total Price with button "Place Order</t>
+  </si>
+  <si>
+    <t>Click "Delete" button at the table of any product</t>
+  </si>
+  <si>
+    <t>Click at "Place Order" button</t>
+  </si>
+  <si>
+    <t>Opens a window to fill delivery and payment information</t>
+  </si>
+  <si>
+    <t>Click "Purchase" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows a warning that tells "Please fill out Name and CreditCard" </t>
+  </si>
+  <si>
+    <t>Fill "Name" and "Credit Card" textboxes and click "Purchase" button</t>
+  </si>
+  <si>
+    <t>Shows an "OK" window with Purchase ID, Amount, Card Number, Name and Date</t>
+  </si>
+  <si>
+    <t>Press "OK" button</t>
+  </si>
+  <si>
+    <t>Website tranfers to the home page</t>
   </si>
 </sst>
 </file>
@@ -683,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -799,6 +884,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1013,6 +1104,345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431C524F-C30A-49E6-89B6-753343DAA184}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{FD98449A-059E-4FB3-A859-8EB3CAA92678}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{B1BECDC0-C1AA-42D3-B088-C2B20D09A92D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1020,7 +1450,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:H34"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1365,15 +1795,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1530,7 +1960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40">
         <v>1</v>
       </c>
@@ -1546,7 +1976,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="41"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40">
         <v>2</v>
       </c>
@@ -1557,7 +1987,7 @@
       <c r="D12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="41"/>
@@ -1712,4 +2142,1087 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E0190E-47EC-44AE-BA15-D01C7ADF82BE}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{724160D9-26A3-42A9-B07A-39239621B90E}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{815C512B-5B14-47FE-B587-C22B51F37A45}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11DD39E-2A6A-48DB-AE66-21EFBDC406A2}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{0CDC3DC8-09FA-4811-B071-6A4F156ACF7A}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{B1296A72-2EE2-4BEF-ADBE-C94233D02C38}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7189C2E-A0E7-4E66-B440-9085FFD4FDBF}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{FCF3A2FE-3008-4ADC-B020-B4CA7358369B}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{2324E0E7-EFF2-4667-81E5-498D28277102}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Log in, sign up test cases
</commit_message>
<xml_diff>
--- a/aqa-inforce-testcases.xlsx
+++ b/aqa-inforce-testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\aqa-inforce-anton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1291ABCE-262E-4132-89B9-47D8C3C16C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E35A9-D783-48F0-BA84-31C8BEE457B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17520" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17520" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC00_Empty" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="TC03_ProductCards" sheetId="4" r:id="rId4"/>
     <sheet name="TC04_UpdatingCart" sheetId="5" r:id="rId5"/>
     <sheet name="TC05_PlacingOrder" sheetId="6" r:id="rId6"/>
+    <sheet name="TC06_SignUp" sheetId="7" r:id="rId7"/>
+    <sheet name="TC07_Login" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -247,6 +249,72 @@
   </si>
   <si>
     <t>Website tranfers to the home page</t>
+  </si>
+  <si>
+    <t>Sign up creating a user account</t>
+  </si>
+  <si>
+    <t>Click "Sign Up" button at navigational panel</t>
+  </si>
+  <si>
+    <t>Opens a "Sign Up" window</t>
+  </si>
+  <si>
+    <t>Click "Sign Up" button at the bottom of the window</t>
+  </si>
+  <si>
+    <t>Shows a subwindow with text "Please fill out Username and Password"</t>
+  </si>
+  <si>
+    <t>Empty Username textbox and fill Password textbox and press "Sign Up" button</t>
+  </si>
+  <si>
+    <t>Fill Username textbox and press "Sign Up" button</t>
+  </si>
+  <si>
+    <t>Fill Username textbox that is already registered and press "Sign Up" button</t>
+  </si>
+  <si>
+    <t>Shows a subwindow "This user already exist"</t>
+  </si>
+  <si>
+    <t>Fill Username textbox that is not registered and press "Sign Up" button</t>
+  </si>
+  <si>
+    <t>Shows a subwindow "Sign up succsesfull"</t>
+  </si>
+  <si>
+    <t>Click "Log In" button at navigational panel</t>
+  </si>
+  <si>
+    <t>Opens a "Log In" window</t>
+  </si>
+  <si>
+    <t>Click "Log In" button at the bottom of the window</t>
+  </si>
+  <si>
+    <t>Fill Username textbox and press "Log In" button</t>
+  </si>
+  <si>
+    <t>Empty Username textbox and fill Password textbox and press "Log In" button</t>
+  </si>
+  <si>
+    <t>Fill Username textbox that is already registered with incorrect password press "Log In" button</t>
+  </si>
+  <si>
+    <t>Shows a subwindow "Wrong password"</t>
+  </si>
+  <si>
+    <t>Fill Username textbox that is already registered with correct password, press "Log In" button</t>
+  </si>
+  <si>
+    <t>Login succesfull. Page updates and Navigation Panel shows "Welcome {username}" and "Log out" button</t>
+  </si>
+  <si>
+    <t>Click "Log Out" button at navigational panel</t>
+  </si>
+  <si>
+    <t>Log out succesfull and website returns to the default state</t>
   </si>
 </sst>
 </file>
@@ -2865,7 +2933,7 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -3225,4 +3293,736 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74A92A6-9752-481F-BEB5-610CB8E7E838}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{1AE1DA4A-1D8F-4D37-9F0A-555DBBB1DD25}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{385E2188-17D3-4BE5-80AA-94ED19C2440F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25930E26-51DB-44B1-ACB5-A2C89C1C5E0F}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="40">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="43"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>45499</v>
+      </c>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{637A9EB0-1AB8-43ED-BFF5-25FBBB3EC989}">
+      <formula1>"Critical,High,Medium,Low"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{D30654C8-7076-41A9-B5E8-4812F0704FFC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>